<commit_message>
updating code to github
</commit_message>
<xml_diff>
--- a/quadrat_data_sheets/all_data_quadrats.xlsx
+++ b/quadrat_data_sheets/all_data_quadrats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s2175119_ed_ac_uk/Documents/uni year 4/dissertation/dissertation/quadrat_data_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="249" documentId="8_{BF7FF229-960D-4661-9D6E-E485E06A770F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77D13AF4-DAEC-4FC7-A5D7-4F358758E229}"/>
+  <xr:revisionPtr revIDLastSave="303" documentId="8_{BF7FF229-960D-4661-9D6E-E485E06A770F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{102983D8-1518-42F3-AED0-F91368473ADF}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7270" xr2:uid="{CC2B858C-F0CC-47E7-86C8-83FFA6CC242D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CC2B858C-F0CC-47E7-86C8-83FFA6CC242D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="287">
   <si>
     <t>date</t>
   </si>
@@ -401,39 +401,15 @@
     <t>veg_species_list</t>
   </si>
   <si>
-    <t>ulva lactua, usnea</t>
-  </si>
-  <si>
     <t>fucus vesiculosus</t>
   </si>
   <si>
     <t>fucus spiralis</t>
   </si>
   <si>
-    <t>fucus spiralis, usnea, ulva lactua, chondrus crispus</t>
-  </si>
-  <si>
-    <t>usnea, laminaria digitata, ulva lactua, corallina officinalis</t>
-  </si>
-  <si>
-    <t>fucus spiralis, usnea, ulva lactua</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>fucus spiralis, usnea, laminaria digitata, ulva lactua, chondrus crispus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">usnea, ulva lactua, corallina officinalis </t>
-  </si>
-  <si>
     <t>pelvetia canaliculata, fucus spiralis</t>
   </si>
   <si>
-    <t xml:space="preserve">none </t>
-  </si>
-  <si>
     <t>ulva lactua, fucus spiralis, chondrus crispus</t>
   </si>
   <si>
@@ -446,12 +422,6 @@
     <t>fucus spiralis, fucus vesiculosus</t>
   </si>
   <si>
-    <t>ulva lactua, fucus spiralis, fucus vesiculosus, usnea</t>
-  </si>
-  <si>
-    <t>pelvetia canaliculata, fucus vesiculosus, ulva lactua, usnea</t>
-  </si>
-  <si>
     <t>ulva lactua</t>
   </si>
   <si>
@@ -464,24 +434,6 @@
     <t>pelvetia canaliculata, fucus vesiculosus, ulva lactua</t>
   </si>
   <si>
-    <t>usnea, pelvetia canaliculata, ulva lactua, corallina officinalis</t>
-  </si>
-  <si>
-    <t>usnea, fucus spiralis, ulva lactua</t>
-  </si>
-  <si>
-    <t>fucus spiralis, usnea</t>
-  </si>
-  <si>
-    <t>usnea, ulva lactua, corallina officinalis</t>
-  </si>
-  <si>
-    <t>usnea</t>
-  </si>
-  <si>
-    <t>usnea, fucus spiralis</t>
-  </si>
-  <si>
     <t>fucus spiralis, ulva lactua</t>
   </si>
   <si>
@@ -512,24 +464,12 @@
     <t>ulva lactua, ascophyllum nodosum, pelvetia canaliculata</t>
   </si>
   <si>
-    <t>usnea, ulva lactua</t>
-  </si>
-  <si>
-    <t>fucus spiralis, usnea, corallina officinalis</t>
-  </si>
-  <si>
     <t xml:space="preserve">fucus spiralis </t>
   </si>
   <si>
-    <t>usnea, fucus spiralis, chondrus crispus</t>
-  </si>
-  <si>
     <t>fucus spiralis, fucus vesiculosus, pelvetia canaliculata</t>
   </si>
   <si>
-    <t>fucus vesiculosus, pelvetia canaliculata, usnea</t>
-  </si>
-  <si>
     <t>ascophyllum nodosum, fucus vesiculosus</t>
   </si>
   <si>
@@ -542,12 +482,6 @@
     <t>ulva lactua, fucus spiralis, ascophyllum nodosum</t>
   </si>
   <si>
-    <t>fucus spiralis, usnea, pelvetia canaliculata, laminaria digitata, ulva lactua, chondrus crispus</t>
-  </si>
-  <si>
-    <t>fucus spiralis, usnea, laminaria digitata, ulva lactua, chondrus crispus, corallina officinalis</t>
-  </si>
-  <si>
     <t xml:space="preserve">pelvetia canaliculata, ulva lactua, fucus spiralis </t>
   </si>
   <si>
@@ -560,30 +494,12 @@
     <t>fucus spiralis, pelvetia canaliculata, fucus vesiculosus</t>
   </si>
   <si>
-    <t>ulva lactua, usnea, fucus spiralis, pelvetia canaliculata</t>
-  </si>
-  <si>
     <t>pelvetia canaliculata, fucus spiralis, fucus vesiculosus, ulva lactua</t>
   </si>
   <si>
     <t>pelvetia canaliculata, ulva lactua, fucus spiralis, chondrus crispus</t>
   </si>
   <si>
-    <t>usnea, fucus spiralis, laminaria digitata, corallina officinalis</t>
-  </si>
-  <si>
-    <t>usnea, pelvetia canaliculata, laminaria digitata, ulva lactua</t>
-  </si>
-  <si>
-    <t>usnea, fucus spiralis, laminaria digitata, ulva lactua, corallina officinalis</t>
-  </si>
-  <si>
-    <t>usnea, fucus spiralis, ulva lactua, laminaria digitata, corallina officinalis</t>
-  </si>
-  <si>
-    <t>fucus spiralis, pelvetia canaliculata, usnea, ulva lactua, laminaria digitata</t>
-  </si>
-  <si>
     <t>fucus vesiculosus, fucus spiralis</t>
   </si>
   <si>
@@ -900,6 +816,87 @@
   </si>
   <si>
     <t>laugh.kilowatt.remodels</t>
+  </si>
+  <si>
+    <t>fucus spiralis, usnea spp.</t>
+  </si>
+  <si>
+    <t>fucus spiralis, usnea spp., pelvetia canaliculata, laminaria digitata, ulva lactua, chondrus crispus</t>
+  </si>
+  <si>
+    <t>fucus spiralis, usnea spp., laminaria digitata, ulva lactua, chondrus crispus, corallina officinalis</t>
+  </si>
+  <si>
+    <t>fucus spiralis, usnea spp., ulva lactua, chondrus crispus</t>
+  </si>
+  <si>
+    <t>usnea spp., laminaria digitata, ulva lactua, corallina officinalis</t>
+  </si>
+  <si>
+    <t>fucus spiralis, usnea spp., ulva lactua</t>
+  </si>
+  <si>
+    <t>no macroalgae present</t>
+  </si>
+  <si>
+    <t>fucus spiralis, usnea spp., laminaria digitata, ulva lactua, chondrus crispus</t>
+  </si>
+  <si>
+    <t>ulva lactua, fucus spiralis, fucus vesiculosus, usnea spp.</t>
+  </si>
+  <si>
+    <t>pelvetia canaliculata, fucus vesiculosus, ulva lactua, usnea spp.</t>
+  </si>
+  <si>
+    <t>usnea spp., pelvetia canaliculata, laminaria digitata, ulva lactua</t>
+  </si>
+  <si>
+    <t>usnea spp., pelvetia canaliculata, ulva lactua, corallina officinalis</t>
+  </si>
+  <si>
+    <t>usnea spp., fucus spiralis, laminaria digitata, ulva lactua, corallina officinalis</t>
+  </si>
+  <si>
+    <t>usnea spp., fucus spiralis, ulva lactua, laminaria digitata, corallina officinalis</t>
+  </si>
+  <si>
+    <t>usnea spp., fucus spiralis, ulva lactua</t>
+  </si>
+  <si>
+    <t>fucus spiralis, pelvetia canaliculata, usnea spp., ulva lactua, laminaria digitata</t>
+  </si>
+  <si>
+    <t>usnea spp.</t>
+  </si>
+  <si>
+    <t>usnea spp., fucus spiralis</t>
+  </si>
+  <si>
+    <t>ulva lactua, usnea spp.</t>
+  </si>
+  <si>
+    <t>ulva lactua, usnea spp., fucus spiralis, pelvetia canaliculata</t>
+  </si>
+  <si>
+    <t>usnea spp., ulva lactua</t>
+  </si>
+  <si>
+    <t>usnea spp., fucus spiralis, laminaria digitata, corallina officinalis</t>
+  </si>
+  <si>
+    <t>fucus spiralis, usnea spp., corallina officinalis</t>
+  </si>
+  <si>
+    <t>usnea spp., fucus spiralis, chondrus crispus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usnea spp., ulva lactua, corallina officinalis </t>
+  </si>
+  <si>
+    <t>fucus vesiculosus, pelvetia canaliculata, usnea spp.</t>
+  </si>
+  <si>
+    <t>usnea spp., ulva lactua, corallina officinalis</t>
   </si>
 </sst>
 </file>
@@ -1277,8 +1274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF1ACB8-2EFF-4506-A58D-5651D06124FB}">
   <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="I2" zoomScale="189" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1302,7 +1299,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1331,7 +1328,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -1349,7 +1346,7 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>144</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1360,7 +1357,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>185</v>
+        <v>157</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -1378,7 +1375,7 @@
         <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>168</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -1389,7 +1386,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -1407,7 +1404,7 @@
         <v>10</v>
       </c>
       <c r="I4" t="s">
-        <v>169</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -1418,7 +1415,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -1436,7 +1433,7 @@
         <v>10</v>
       </c>
       <c r="I5" t="s">
-        <v>124</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -1447,7 +1444,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -1465,7 +1462,7 @@
         <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>125</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -1476,7 +1473,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
@@ -1494,7 +1491,7 @@
         <v>10</v>
       </c>
       <c r="I7" t="s">
-        <v>126</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -1505,7 +1502,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -1523,7 +1520,7 @@
         <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -1534,7 +1531,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
@@ -1552,7 +1549,7 @@
         <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1563,7 +1560,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
@@ -1581,7 +1578,7 @@
         <v>10</v>
       </c>
       <c r="I10" t="s">
-        <v>128</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1592,7 +1589,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
@@ -1610,7 +1607,7 @@
         <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>129</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1621,7 +1618,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
@@ -1639,7 +1636,7 @@
         <v>10</v>
       </c>
       <c r="I12" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -1650,7 +1647,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -1668,7 +1665,7 @@
         <v>10</v>
       </c>
       <c r="I13" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1679,7 +1676,7 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="D14" t="s">
         <v>23</v>
@@ -1697,7 +1694,7 @@
         <v>10</v>
       </c>
       <c r="I14" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -1708,7 +1705,7 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>197</v>
+        <v>169</v>
       </c>
       <c r="D15" t="s">
         <v>24</v>
@@ -1726,7 +1723,7 @@
         <v>10</v>
       </c>
       <c r="I15" t="s">
-        <v>176</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -1737,7 +1734,7 @@
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="D16" t="s">
         <v>25</v>
@@ -1755,7 +1752,7 @@
         <v>10</v>
       </c>
       <c r="I16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1766,7 +1763,7 @@
         <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="D17" t="s">
         <v>26</v>
@@ -1784,7 +1781,7 @@
         <v>10</v>
       </c>
       <c r="I17" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -1795,7 +1792,7 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>200</v>
+        <v>172</v>
       </c>
       <c r="D18" t="s">
         <v>27</v>
@@ -1813,7 +1810,7 @@
         <v>10</v>
       </c>
       <c r="I18" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1824,7 +1821,7 @@
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>201</v>
+        <v>173</v>
       </c>
       <c r="D19" t="s">
         <v>28</v>
@@ -1842,7 +1839,7 @@
         <v>10</v>
       </c>
       <c r="I19" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -1853,7 +1850,7 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="D20" t="s">
         <v>26</v>
@@ -1871,7 +1868,7 @@
         <v>10</v>
       </c>
       <c r="I20" t="s">
-        <v>131</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -1882,7 +1879,7 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>202</v>
+        <v>174</v>
       </c>
       <c r="D21" t="s">
         <v>29</v>
@@ -1900,7 +1897,7 @@
         <v>10</v>
       </c>
       <c r="I21" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -1911,7 +1908,7 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>203</v>
+        <v>175</v>
       </c>
       <c r="D22" t="s">
         <v>30</v>
@@ -1929,7 +1926,7 @@
         <v>10</v>
       </c>
       <c r="I22" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1940,7 +1937,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>204</v>
+        <v>176</v>
       </c>
       <c r="D23" t="s">
         <v>31</v>
@@ -1958,7 +1955,7 @@
         <v>10</v>
       </c>
       <c r="I23" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -1969,7 +1966,7 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>205</v>
+        <v>177</v>
       </c>
       <c r="D24" t="s">
         <v>32</v>
@@ -1987,7 +1984,7 @@
         <v>10</v>
       </c>
       <c r="I24" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -1998,7 +1995,7 @@
         <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>206</v>
+        <v>178</v>
       </c>
       <c r="D25" t="s">
         <v>33</v>
@@ -2016,7 +2013,7 @@
         <v>10</v>
       </c>
       <c r="I25" t="s">
-        <v>136</v>
+        <v>268</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -2027,7 +2024,7 @@
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>207</v>
+        <v>179</v>
       </c>
       <c r="D26" t="s">
         <v>34</v>
@@ -2045,7 +2042,7 @@
         <v>10</v>
       </c>
       <c r="I26" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -2056,7 +2053,7 @@
         <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
       <c r="D27" t="s">
         <v>37</v>
@@ -2074,7 +2071,7 @@
         <v>10</v>
       </c>
       <c r="I27" t="s">
-        <v>137</v>
+        <v>269</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -2085,7 +2082,7 @@
         <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>209</v>
+        <v>181</v>
       </c>
       <c r="D28" t="s">
         <v>38</v>
@@ -2103,7 +2100,7 @@
         <v>10</v>
       </c>
       <c r="I28" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -2114,7 +2111,7 @@
         <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="D29" t="s">
         <v>39</v>
@@ -2132,7 +2129,7 @@
         <v>10</v>
       </c>
       <c r="I29" t="s">
-        <v>137</v>
+        <v>269</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
@@ -2143,7 +2140,7 @@
         <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
       <c r="D30" t="s">
         <v>40</v>
@@ -2161,7 +2158,7 @@
         <v>10</v>
       </c>
       <c r="I30" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
@@ -2172,7 +2169,7 @@
         <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="D31" t="s">
         <v>41</v>
@@ -2190,7 +2187,7 @@
         <v>10</v>
       </c>
       <c r="I31" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
@@ -2201,7 +2198,7 @@
         <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>213</v>
+        <v>185</v>
       </c>
       <c r="D32" t="s">
         <v>42</v>
@@ -2219,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="I32" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
@@ -2230,7 +2227,7 @@
         <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="D33" t="s">
         <v>43</v>
@@ -2248,7 +2245,7 @@
         <v>10</v>
       </c>
       <c r="I33" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
@@ -2259,7 +2256,7 @@
         <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
       <c r="D34" t="s">
         <v>44</v>
@@ -2277,7 +2274,7 @@
         <v>10</v>
       </c>
       <c r="I34" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
@@ -2288,7 +2285,7 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>216</v>
+        <v>188</v>
       </c>
       <c r="D35" t="s">
         <v>45</v>
@@ -2306,7 +2303,7 @@
         <v>10</v>
       </c>
       <c r="I35" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.35">
@@ -2317,7 +2314,7 @@
         <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>217</v>
+        <v>189</v>
       </c>
       <c r="D36" t="s">
         <v>46</v>
@@ -2335,7 +2332,7 @@
         <v>10</v>
       </c>
       <c r="I36" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.35">
@@ -2346,7 +2343,7 @@
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
       <c r="D37" t="s">
         <v>48</v>
@@ -2364,7 +2361,7 @@
         <v>10</v>
       </c>
       <c r="I37" t="s">
-        <v>178</v>
+        <v>270</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
@@ -2375,7 +2372,7 @@
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
       <c r="D38" t="s">
         <v>49</v>
@@ -2393,7 +2390,7 @@
         <v>10</v>
       </c>
       <c r="I38" t="s">
-        <v>142</v>
+        <v>271</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
@@ -2404,7 +2401,7 @@
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="D39" t="s">
         <v>50</v>
@@ -2422,7 +2419,7 @@
         <v>10</v>
       </c>
       <c r="I39" t="s">
-        <v>179</v>
+        <v>272</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -2433,7 +2430,7 @@
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>221</v>
+        <v>193</v>
       </c>
       <c r="D40" t="s">
         <v>51</v>
@@ -2451,7 +2448,7 @@
         <v>10</v>
       </c>
       <c r="I40" t="s">
-        <v>179</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
@@ -2462,7 +2459,7 @@
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>222</v>
+        <v>194</v>
       </c>
       <c r="D41" t="s">
         <v>52</v>
@@ -2480,7 +2477,7 @@
         <v>10</v>
       </c>
       <c r="I41" t="s">
-        <v>180</v>
+        <v>273</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
@@ -2491,7 +2488,7 @@
         <v>8</v>
       </c>
       <c r="C42" t="s">
-        <v>223</v>
+        <v>195</v>
       </c>
       <c r="D42" t="s">
         <v>53</v>
@@ -2509,7 +2506,7 @@
         <v>10</v>
       </c>
       <c r="I42" t="s">
-        <v>143</v>
+        <v>274</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
@@ -2520,7 +2517,7 @@
         <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>224</v>
+        <v>196</v>
       </c>
       <c r="D43" t="s">
         <v>54</v>
@@ -2538,7 +2535,7 @@
         <v>10</v>
       </c>
       <c r="I43" t="s">
-        <v>181</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -2549,7 +2546,7 @@
         <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>225</v>
+        <v>197</v>
       </c>
       <c r="D44" t="s">
         <v>55</v>
@@ -2567,7 +2564,7 @@
         <v>10</v>
       </c>
       <c r="I44" t="s">
-        <v>144</v>
+        <v>260</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -2578,7 +2575,7 @@
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>226</v>
+        <v>198</v>
       </c>
       <c r="D45" t="s">
         <v>56</v>
@@ -2596,7 +2593,7 @@
         <v>10</v>
       </c>
       <c r="I45" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
@@ -2607,7 +2604,7 @@
         <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>227</v>
+        <v>199</v>
       </c>
       <c r="D46" t="s">
         <v>57</v>
@@ -2625,7 +2622,7 @@
         <v>10</v>
       </c>
       <c r="I46" t="s">
-        <v>145</v>
+        <v>286</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
@@ -2636,7 +2633,7 @@
         <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>228</v>
+        <v>200</v>
       </c>
       <c r="D47" t="s">
         <v>58</v>
@@ -2654,7 +2651,7 @@
         <v>10</v>
       </c>
       <c r="I47" t="s">
-        <v>146</v>
+        <v>276</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
@@ -2665,7 +2662,7 @@
         <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
       <c r="D48" t="s">
         <v>59</v>
@@ -2683,7 +2680,7 @@
         <v>10</v>
       </c>
       <c r="I48" t="s">
-        <v>147</v>
+        <v>277</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
@@ -2694,7 +2691,7 @@
         <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>230</v>
+        <v>202</v>
       </c>
       <c r="D49" t="s">
         <v>60</v>
@@ -2712,7 +2709,7 @@
         <v>10</v>
       </c>
       <c r="I49" t="s">
-        <v>146</v>
+        <v>276</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
@@ -2723,7 +2720,7 @@
         <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>231</v>
+        <v>203</v>
       </c>
       <c r="D50" t="s">
         <v>61</v>
@@ -2741,7 +2738,7 @@
         <v>10</v>
       </c>
       <c r="I50" t="s">
-        <v>121</v>
+        <v>278</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
@@ -2752,7 +2749,7 @@
         <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>232</v>
+        <v>204</v>
       </c>
       <c r="D51" t="s">
         <v>62</v>
@@ -2770,7 +2767,7 @@
         <v>10</v>
       </c>
       <c r="I51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
@@ -2781,7 +2778,7 @@
         <v>22</v>
       </c>
       <c r="C52" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="D52" t="s">
         <v>63</v>
@@ -2799,7 +2796,7 @@
         <v>10</v>
       </c>
       <c r="I52" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
@@ -2810,7 +2807,7 @@
         <v>22</v>
       </c>
       <c r="C53" t="s">
-        <v>234</v>
+        <v>206</v>
       </c>
       <c r="D53" t="s">
         <v>64</v>
@@ -2828,7 +2825,7 @@
         <v>10</v>
       </c>
       <c r="I53" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
@@ -2839,7 +2836,7 @@
         <v>22</v>
       </c>
       <c r="C54" t="s">
-        <v>235</v>
+        <v>207</v>
       </c>
       <c r="D54" t="s">
         <v>65</v>
@@ -2857,7 +2854,7 @@
         <v>10</v>
       </c>
       <c r="I54" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
@@ -2868,7 +2865,7 @@
         <v>22</v>
       </c>
       <c r="C55" t="s">
-        <v>236</v>
+        <v>208</v>
       </c>
       <c r="D55" t="s">
         <v>66</v>
@@ -2886,7 +2883,7 @@
         <v>10</v>
       </c>
       <c r="I55" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
@@ -2897,7 +2894,7 @@
         <v>22</v>
       </c>
       <c r="C56" t="s">
-        <v>237</v>
+        <v>209</v>
       </c>
       <c r="D56" t="s">
         <v>67</v>
@@ -2915,7 +2912,7 @@
         <v>10</v>
       </c>
       <c r="I56" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
@@ -2926,7 +2923,7 @@
         <v>22</v>
       </c>
       <c r="C57" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="D57" t="s">
         <v>68</v>
@@ -2944,7 +2941,7 @@
         <v>10</v>
       </c>
       <c r="I57" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
@@ -2955,7 +2952,7 @@
         <v>22</v>
       </c>
       <c r="C58" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="D58" t="s">
         <v>69</v>
@@ -2973,7 +2970,7 @@
         <v>10</v>
       </c>
       <c r="I58" t="s">
-        <v>131</v>
+        <v>266</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
@@ -2984,7 +2981,7 @@
         <v>22</v>
       </c>
       <c r="C59" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="D59" t="s">
         <v>70</v>
@@ -3002,7 +2999,7 @@
         <v>10</v>
       </c>
       <c r="I59" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
@@ -3013,7 +3010,7 @@
         <v>22</v>
       </c>
       <c r="C60" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
       <c r="D60" t="s">
         <v>71</v>
@@ -3031,7 +3028,7 @@
         <v>72</v>
       </c>
       <c r="I60" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
@@ -3042,7 +3039,7 @@
         <v>22</v>
       </c>
       <c r="C61" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="D61" t="s">
         <v>73</v>
@@ -3060,7 +3057,7 @@
         <v>10</v>
       </c>
       <c r="I61" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
@@ -3071,7 +3068,7 @@
         <v>22</v>
       </c>
       <c r="C62" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="D62" t="s">
         <v>74</v>
@@ -3089,7 +3086,7 @@
         <v>10</v>
       </c>
       <c r="I62" t="s">
-        <v>174</v>
+        <v>279</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
@@ -3100,7 +3097,7 @@
         <v>22</v>
       </c>
       <c r="C63" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
       <c r="D63" t="s">
         <v>75</v>
@@ -3118,7 +3115,7 @@
         <v>10</v>
       </c>
       <c r="I63" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
@@ -3129,7 +3126,7 @@
         <v>22</v>
       </c>
       <c r="C64" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
       <c r="D64" t="s">
         <v>76</v>
@@ -3147,7 +3144,7 @@
         <v>10</v>
       </c>
       <c r="I64" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.35">
@@ -3158,7 +3155,7 @@
         <v>22</v>
       </c>
       <c r="C65" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
       <c r="D65" t="s">
         <v>77</v>
@@ -3176,7 +3173,7 @@
         <v>10</v>
       </c>
       <c r="I65" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.35">
@@ -3187,7 +3184,7 @@
         <v>22</v>
       </c>
       <c r="C66" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="D66" t="s">
         <v>78</v>
@@ -3205,7 +3202,7 @@
         <v>10</v>
       </c>
       <c r="I66" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.35">
@@ -3216,7 +3213,7 @@
         <v>36</v>
       </c>
       <c r="C67" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
       <c r="D67" t="s">
         <v>79</v>
@@ -3234,7 +3231,7 @@
         <v>10</v>
       </c>
       <c r="I67" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.35">
@@ -3245,7 +3242,7 @@
         <v>36</v>
       </c>
       <c r="C68" t="s">
-        <v>249</v>
+        <v>221</v>
       </c>
       <c r="D68" t="s">
         <v>80</v>
@@ -3263,7 +3260,7 @@
         <v>10</v>
       </c>
       <c r="I68" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
@@ -3274,7 +3271,7 @@
         <v>36</v>
       </c>
       <c r="C69" t="s">
-        <v>250</v>
+        <v>222</v>
       </c>
       <c r="D69" t="s">
         <v>81</v>
@@ -3292,7 +3289,7 @@
         <v>10</v>
       </c>
       <c r="I69" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
@@ -3303,7 +3300,7 @@
         <v>36</v>
       </c>
       <c r="C70" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="D70" t="s">
         <v>82</v>
@@ -3321,7 +3318,7 @@
         <v>10</v>
       </c>
       <c r="I70" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.35">
@@ -3332,7 +3329,7 @@
         <v>36</v>
       </c>
       <c r="C71" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="D71" t="s">
         <v>83</v>
@@ -3350,7 +3347,7 @@
         <v>72</v>
       </c>
       <c r="I71" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
@@ -3361,7 +3358,7 @@
         <v>36</v>
       </c>
       <c r="C72" t="s">
-        <v>253</v>
+        <v>225</v>
       </c>
       <c r="D72" t="s">
         <v>84</v>
@@ -3379,7 +3376,7 @@
         <v>10</v>
       </c>
       <c r="I72" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
@@ -3390,7 +3387,7 @@
         <v>36</v>
       </c>
       <c r="C73" t="s">
-        <v>254</v>
+        <v>226</v>
       </c>
       <c r="D73" t="s">
         <v>85</v>
@@ -3408,7 +3405,7 @@
         <v>10</v>
       </c>
       <c r="I73" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -3419,7 +3416,7 @@
         <v>36</v>
       </c>
       <c r="C74" t="s">
-        <v>255</v>
+        <v>227</v>
       </c>
       <c r="D74" t="s">
         <v>86</v>
@@ -3437,7 +3434,7 @@
         <v>10</v>
       </c>
       <c r="I74" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.35">
@@ -3448,7 +3445,7 @@
         <v>36</v>
       </c>
       <c r="C75" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
       <c r="D75" t="s">
         <v>87</v>
@@ -3466,7 +3463,7 @@
         <v>10</v>
       </c>
       <c r="I75" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.35">
@@ -3477,7 +3474,7 @@
         <v>36</v>
       </c>
       <c r="C76" t="s">
-        <v>257</v>
+        <v>229</v>
       </c>
       <c r="D76" t="s">
         <v>88</v>
@@ -3495,7 +3492,7 @@
         <v>10</v>
       </c>
       <c r="I76" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
@@ -3506,7 +3503,7 @@
         <v>8</v>
       </c>
       <c r="C77" t="s">
-        <v>258</v>
+        <v>230</v>
       </c>
       <c r="D77" t="s">
         <v>90</v>
@@ -3524,7 +3521,7 @@
         <v>10</v>
       </c>
       <c r="I77" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.35">
@@ -3535,7 +3532,7 @@
         <v>8</v>
       </c>
       <c r="C78" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
       <c r="D78" t="s">
         <v>91</v>
@@ -3553,7 +3550,7 @@
         <v>10</v>
       </c>
       <c r="I78" t="s">
-        <v>158</v>
+        <v>280</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.35">
@@ -3564,7 +3561,7 @@
         <v>8</v>
       </c>
       <c r="C79" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
       <c r="D79" t="s">
         <v>92</v>
@@ -3582,7 +3579,7 @@
         <v>10</v>
       </c>
       <c r="I79" t="s">
-        <v>177</v>
+        <v>281</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
@@ -3593,7 +3590,7 @@
         <v>8</v>
       </c>
       <c r="C80" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
       <c r="D80" t="s">
         <v>93</v>
@@ -3611,7 +3608,7 @@
         <v>10</v>
       </c>
       <c r="I80" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
@@ -3622,7 +3619,7 @@
         <v>8</v>
       </c>
       <c r="C81" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="D81" t="s">
         <v>94</v>
@@ -3640,7 +3637,7 @@
         <v>10</v>
       </c>
       <c r="I81" t="s">
-        <v>159</v>
+        <v>282</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.35">
@@ -3651,7 +3648,7 @@
         <v>8</v>
       </c>
       <c r="C82" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D82" t="s">
         <v>95</v>
@@ -3669,7 +3666,7 @@
         <v>10</v>
       </c>
       <c r="I82" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.35">
@@ -3680,7 +3677,7 @@
         <v>8</v>
       </c>
       <c r="C83" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D83" t="s">
         <v>96</v>
@@ -3698,7 +3695,7 @@
         <v>10</v>
       </c>
       <c r="I83" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.35">
@@ -3709,7 +3706,7 @@
         <v>8</v>
       </c>
       <c r="C84" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
       <c r="D84" t="s">
         <v>97</v>
@@ -3727,7 +3724,7 @@
         <v>10</v>
       </c>
       <c r="I84" t="s">
-        <v>144</v>
+        <v>260</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.35">
@@ -3738,7 +3735,7 @@
         <v>8</v>
       </c>
       <c r="C85" t="s">
-        <v>266</v>
+        <v>238</v>
       </c>
       <c r="D85" t="s">
         <v>98</v>
@@ -3756,7 +3753,7 @@
         <v>10</v>
       </c>
       <c r="I85" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.35">
@@ -3767,7 +3764,7 @@
         <v>8</v>
       </c>
       <c r="C86" t="s">
-        <v>267</v>
+        <v>239</v>
       </c>
       <c r="D86" t="s">
         <v>99</v>
@@ -3785,7 +3782,7 @@
         <v>10</v>
       </c>
       <c r="I86" t="s">
-        <v>159</v>
+        <v>282</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.35">
@@ -3796,7 +3793,7 @@
         <v>8</v>
       </c>
       <c r="C87" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="D87" t="s">
         <v>100</v>
@@ -3814,7 +3811,7 @@
         <v>10</v>
       </c>
       <c r="I87" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.35">
@@ -3825,7 +3822,7 @@
         <v>22</v>
       </c>
       <c r="C88" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
       <c r="D88" t="s">
         <v>101</v>
@@ -3843,7 +3840,7 @@
         <v>10</v>
       </c>
       <c r="I88" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
@@ -3854,7 +3851,7 @@
         <v>22</v>
       </c>
       <c r="C89" t="s">
-        <v>270</v>
+        <v>242</v>
       </c>
       <c r="D89" t="s">
         <v>102</v>
@@ -3872,7 +3869,7 @@
         <v>10</v>
       </c>
       <c r="I89" t="s">
-        <v>161</v>
+        <v>283</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.35">
@@ -3883,7 +3880,7 @@
         <v>22</v>
       </c>
       <c r="C90" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="D90" t="s">
         <v>74</v>
@@ -3901,7 +3898,7 @@
         <v>10</v>
       </c>
       <c r="I90" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
@@ -3912,7 +3909,7 @@
         <v>22</v>
       </c>
       <c r="C91" t="s">
-        <v>271</v>
+        <v>243</v>
       </c>
       <c r="D91" t="s">
         <v>103</v>
@@ -3930,7 +3927,7 @@
         <v>10</v>
       </c>
       <c r="I91" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.35">
@@ -3941,7 +3938,7 @@
         <v>22</v>
       </c>
       <c r="C92" t="s">
-        <v>272</v>
+        <v>244</v>
       </c>
       <c r="D92" t="s">
         <v>104</v>
@@ -3959,7 +3956,7 @@
         <v>10</v>
       </c>
       <c r="I92" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.35">
@@ -3970,7 +3967,7 @@
         <v>22</v>
       </c>
       <c r="C93" t="s">
-        <v>273</v>
+        <v>245</v>
       </c>
       <c r="D93" t="s">
         <v>105</v>
@@ -3988,7 +3985,7 @@
         <v>10</v>
       </c>
       <c r="I93" t="s">
-        <v>158</v>
+        <v>280</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.35">
@@ -3999,7 +3996,7 @@
         <v>22</v>
       </c>
       <c r="C94" t="s">
-        <v>274</v>
+        <v>246</v>
       </c>
       <c r="D94" t="s">
         <v>106</v>
@@ -4017,7 +4014,7 @@
         <v>10</v>
       </c>
       <c r="I94" t="s">
-        <v>146</v>
+        <v>276</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
@@ -4028,7 +4025,7 @@
         <v>22</v>
       </c>
       <c r="C95" t="s">
-        <v>275</v>
+        <v>247</v>
       </c>
       <c r="D95" t="s">
         <v>107</v>
@@ -4046,7 +4043,7 @@
         <v>10</v>
       </c>
       <c r="I95" t="s">
-        <v>146</v>
+        <v>276</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
@@ -4057,7 +4054,7 @@
         <v>22</v>
       </c>
       <c r="C96" t="s">
-        <v>276</v>
+        <v>248</v>
       </c>
       <c r="D96" t="s">
         <v>108</v>
@@ -4075,7 +4072,7 @@
         <v>10</v>
       </c>
       <c r="I96" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
@@ -4086,7 +4083,7 @@
         <v>22</v>
       </c>
       <c r="C97" t="s">
-        <v>277</v>
+        <v>249</v>
       </c>
       <c r="D97" t="s">
         <v>109</v>
@@ -4104,7 +4101,7 @@
         <v>10</v>
       </c>
       <c r="I97" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.35">
@@ -4115,7 +4112,7 @@
         <v>36</v>
       </c>
       <c r="C98" t="s">
-        <v>278</v>
+        <v>250</v>
       </c>
       <c r="D98" t="s">
         <v>110</v>
@@ -4133,7 +4130,7 @@
         <v>10</v>
       </c>
       <c r="I98" t="s">
-        <v>163</v>
+        <v>285</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
@@ -4144,7 +4141,7 @@
         <v>36</v>
       </c>
       <c r="C99" t="s">
-        <v>279</v>
+        <v>251</v>
       </c>
       <c r="D99" t="s">
         <v>111</v>
@@ -4162,7 +4159,7 @@
         <v>10</v>
       </c>
       <c r="I99" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
@@ -4173,7 +4170,7 @@
         <v>36</v>
       </c>
       <c r="C100" t="s">
-        <v>280</v>
+        <v>252</v>
       </c>
       <c r="D100" t="s">
         <v>112</v>
@@ -4191,7 +4188,7 @@
         <v>10</v>
       </c>
       <c r="I100" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
@@ -4202,7 +4199,7 @@
         <v>36</v>
       </c>
       <c r="C101" t="s">
-        <v>281</v>
+        <v>253</v>
       </c>
       <c r="D101" t="s">
         <v>113</v>
@@ -4220,7 +4217,7 @@
         <v>10</v>
       </c>
       <c r="I101" t="s">
-        <v>121</v>
+        <v>278</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
@@ -4231,7 +4228,7 @@
         <v>36</v>
       </c>
       <c r="C102" t="s">
-        <v>282</v>
+        <v>254</v>
       </c>
       <c r="D102" t="s">
         <v>114</v>
@@ -4249,7 +4246,7 @@
         <v>10</v>
       </c>
       <c r="I102" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
@@ -4260,7 +4257,7 @@
         <v>36</v>
       </c>
       <c r="C103" t="s">
-        <v>283</v>
+        <v>255</v>
       </c>
       <c r="D103" t="s">
         <v>115</v>
@@ -4278,7 +4275,7 @@
         <v>10</v>
       </c>
       <c r="I103" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
@@ -4289,7 +4286,7 @@
         <v>36</v>
       </c>
       <c r="C104" t="s">
-        <v>284</v>
+        <v>256</v>
       </c>
       <c r="D104" t="s">
         <v>116</v>
@@ -4307,7 +4304,7 @@
         <v>10</v>
       </c>
       <c r="I104" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
@@ -4318,7 +4315,7 @@
         <v>36</v>
       </c>
       <c r="C105" t="s">
-        <v>285</v>
+        <v>257</v>
       </c>
       <c r="D105" t="s">
         <v>117</v>
@@ -4336,7 +4333,7 @@
         <v>72</v>
       </c>
       <c r="I105" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
@@ -4347,7 +4344,7 @@
         <v>36</v>
       </c>
       <c r="C106" t="s">
-        <v>286</v>
+        <v>258</v>
       </c>
       <c r="D106" t="s">
         <v>118</v>
@@ -4365,7 +4362,7 @@
         <v>72</v>
       </c>
       <c r="I106" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.35">
@@ -4376,7 +4373,7 @@
         <v>36</v>
       </c>
       <c r="C107" t="s">
-        <v>287</v>
+        <v>259</v>
       </c>
       <c r="D107" t="s">
         <v>119</v>
@@ -4394,7 +4391,7 @@
         <v>10</v>
       </c>
       <c r="I107" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>